<commit_message>
Added FLexiHAL to list.
</commit_message>
<xml_diff>
--- a/Controllers.xlsx
+++ b/Controllers.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\GRBLHAL_Expatria\Controllers\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="33555" windowHeight="16170"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="49">
   <si>
     <t>Controller</t>
   </si>
@@ -157,6 +162,12 @@
   </si>
   <si>
     <t>[SMART Ramps](https://reprap.org/wiki/SMART_RAMPS)</t>
+  </si>
+  <si>
+    <t>[STM32F4xxhttps://github.com/grblHAL/STM32F4xx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Flexi-HAL](https://github.com/Expatria-Technologies/Flexi-HAL) </t>
   </si>
 </sst>
 </file>
@@ -204,6 +215,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -252,7 +266,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,7 +301,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -496,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -614,47 +628,47 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>48</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
@@ -662,15 +676,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>18</v>
@@ -678,23 +692,23 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>46</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
         <v>20</v>
@@ -702,31 +716,31 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3</v>
+        <v>46</v>
       </c>
       <c r="B25" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>36</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>35</v>
+        <v>2</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B28" t="s">
         <v>40</v>
@@ -734,7 +748,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B29" t="s">
         <v>40</v>
@@ -742,7 +756,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
         <v>40</v>
@@ -750,25 +764,33 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="B31" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B32" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>44</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Mach 3 USB breakout board
</commit_message>
<xml_diff>
--- a/Controllers.xlsx
+++ b/Controllers.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
   <si>
     <t>Controller</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>[STM32F401CCU6 UNI](https://github.com/Am0k-GIT/STM32F401CCU6_UNI)</t>
+  </si>
+  <si>
+    <t>[Mach 3 USB BOB - BSMCE04U-PP](https://drufelcnc.com/?c=controllers&amp;p=BSMCE04U)&lt;sup&gt;1&lt;/sup&gt;</t>
   </si>
 </sst>
 </file>
@@ -508,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,47 +637,47 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>4</v>
+        <v>50</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
@@ -682,23 +685,23 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B21" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B22" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="B23" t="s">
         <v>17</v>
@@ -706,71 +709,71 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="B27" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
+        <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>33</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>49</v>
+        <v>34</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B32" t="s">
         <v>38</v>
@@ -778,7 +781,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
         <v>38</v>
@@ -786,7 +789,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B34" t="s">
         <v>38</v>
@@ -794,23 +797,31 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>31</v>
+      </c>
+      <c r="B36" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>42</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B36">
-    <sortCondition ref="A2:A36"/>
+  <sortState ref="A2:B37">
+    <sortCondition ref="A2:A37"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
git cannot merge so readded file
</commit_message>
<xml_diff>
--- a/Controllers.xlsx
+++ b/Controllers.xlsx
@@ -678,8 +678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updated sienci SLB-EXT product url
</commit_message>
<xml_diff>
--- a/Controllers.xlsx
+++ b/Controllers.xlsx
@@ -1,24 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D002EC2C-B2D2-4FF5-9C6D-03FA6BD07840}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="5850" yWindow="720" windowWidth="44415" windowHeight="31680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="114">
   <si>
     <t>Controller</t>
   </si>
@@ -26,7 +30,7 @@
     <t>Driver</t>
   </si>
   <si>
-    <t xml:space="preserve">[6-Pack CNC Controller](https://github.com/bdring/6-Pack_CNC_Controller)</t>
+    <t>[6-Pack CNC Controller](https://github.com/bdring/6-Pack_CNC_Controller)</t>
   </si>
   <si>
     <t>[ESP32](https://github.com/grblHAL/ESP32)</t>
@@ -35,25 +39,25 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=BDRING%206-axis%20I2S)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Arduino Due](https://store.arduino.cc/arduino-due) with [Arduino Due shield](https://github.com/itadinanta/cnc_mill_prototype/tree/master/arduino_duo_shield)</t>
+    <t>[Arduino Due](https://store.arduino.cc/arduino-due) with [Arduino Due shield](https://github.com/itadinanta/cnc_mill_prototype/tree/master/arduino_duo_shield)</t>
   </si>
   <si>
     <t>[SAM3X8E](https://github.com/grblHAL/SAM3X8E)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Arduino Due](https://store.arduino.cc/arduino-due) with [G2core-DUE-External-Interfaces](https://github.com/cmcgrath5035/G2core-DUE-External-Interfaces)</t>
+    <t>[Arduino Due](https://store.arduino.cc/arduino-due) with [G2core-DUE-External-Interfaces](https://github.com/cmcgrath5035/G2core-DUE-External-Interfaces)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=SAM3X8E&amp;board=cmgrath%20v3)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Arduino Due](https://store.arduino.cc/arduino-due) with [Ramps 1.6](https://reprap.org/wiki/RAMPS_1.6)</t>
+    <t>[Arduino Due](https://store.arduino.cc/arduino-due) with [Ramps 1.6](https://reprap.org/wiki/RAMPS_1.6)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=SAM3X8E&amp;board=Ramps%201.6)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech Octopus MAX 3](https://github.com/bigtreetech/Octopus-Max-EZ)</t>
+    <t>[Bigtreetech Octopus MAX 3](https://github.com/bigtreetech/Octopus-Max-EZ)</t>
   </si>
   <si>
     <t>[STM32H7xx](https://github.com/dresco/STM32H7xx)</t>
@@ -62,19 +66,19 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32H7xx&amp;board=BTT%20Octopus%20MAX%20H723)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech Rodent](https://github.com/bigtreetech/Rodent/tree/master)</t>
+    <t>[Bigtreetech Rodent](https://github.com/bigtreetech/Rodent/tree/master)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=BTT%20Rodent)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech Scylla](https://github.com/bigtreetech/Scylla)</t>
+    <t>[Bigtreetech Scylla](https://github.com/bigtreetech/Scylla)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32H7xx&amp;board=BTT%20Scylla%20H723)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR 2](https://www.bigtree-tech.com/products/bigtreetech-skr-2.html)</t>
+    <t>[Bigtreetech SKR 2](https://www.bigtree-tech.com/products/bigtreetech-skr-2.html)</t>
   </si>
   <si>
     <t>[STM32F4xx](https://github.com/grblHAL/STM32F4xx)</t>
@@ -83,13 +87,13 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=BTT%20SKR-2%20STM32F407)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR 3](https://biqu.equipment/collections/control-board/products/bigtreetech-btt-skr-3-control-board-for-3d-printer)</t>
+    <t>[Bigtreetech SKR 3](https://biqu.equipment/collections/control-board/products/bigtreetech-btt-skr-3-control-board-for-3d-printer)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32H7xx&amp;board=BTT%20SKR%203)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR MINI E3 V2.0](https://www.bigtree-tech.com/products/bigtreetech-skr-mini-e3-v2-0-32-bit-control-board-integrated-tmc2209-uart-for-ender-3.html)</t>
+    <t>[Bigtreetech SKR MINI E3 V2.0](https://www.bigtree-tech.com/products/bigtreetech-skr-mini-e3-v2-0-32-bit-control-board-integrated-tmc2209-uart-for-ender-3.html)</t>
   </si>
   <si>
     <t>[STM32F1xx](https://github.com/grblHAL/STM32F1xx)</t>
@@ -107,34 +111,34 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=RP2040&amp;board=BTT%20SKR%20Pico%201.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR PRO](https://www.bigtree-tech.com/products/bigtreetech-skr-pro-v1-2.html)</t>
+    <t>[Bigtreetech SKR PRO](https://www.bigtree-tech.com/products/bigtreetech-skr-pro-v1-2.html)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=BTT%20SKR%20PRO%20v1.2)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR v1.3](https://duckduckgo.com/?t=ffsb&amp;q=btt+skr+1.3&amp;ia=web)</t>
+    <t>[Bigtreetech SKR v1.3](https://duckduckgo.com/?t=ffsb&amp;q=btt+skr+1.3&amp;ia=web)</t>
   </si>
   <si>
     <t>[LPC176x](https://github.com/grblHAL/LPC176x)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Bigtreetech SKR V1.4 Turbo](https://www.bigtree-tech.com/products/btt-skr-v1-4-skr-v1-4-turbo-32-bit-control-board.html)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[CNC3040](https://github.com/shaise/GrblCNC) with a Red/BluePill</t>
+    <t>[Bigtreetech SKR V1.4 Turbo](https://www.bigtree-tech.com/products/btt-skr-v1-4-skr-v1-4-turbo-32-bit-control-board.html)</t>
+  </si>
+  <si>
+    <t>[CNC3040](https://github.com/shaise/GrblCNC) with a Red/BluePill</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F1xx&amp;board=CNC%203040%20%28Red/Bluepill%20128K%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[EK-TM4C123GXL LaunchPad](https://www.ti.com/tool/EK-TM4C123GXL) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
+    <t>[EK-TM4C123GXL LaunchPad](https://www.ti.com/tool/EK-TM4C123GXL) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
   </si>
   <si>
     <t>[TM4C123](https://github.com/grblHAL/TM4C123)</t>
   </si>
   <si>
-    <t xml:space="preserve">[EK-TM4C1294XL LaunchPad](https://www.ti.com/tool/EK-TM4C1294XL#) with [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
+    <t>[EK-TM4C1294XL LaunchPad](https://www.ti.com/tool/EK-TM4C1294XL#) with [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
   </si>
   <si>
     <t>[TM4C1294](https://github.com/grblHAL/TM4C1294)</t>
@@ -158,100 +162,100 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Flexi-HAL)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Fysetc E4](https://www.fysetc.com/products/fysetc-e4-board-with-built-in-wi-fi-and-bluetooth-4-pcs-tmc2209-240mhz-16m-flash-3d-printer-control-board-based-for-3d-printer?variant=37558333341871)</t>
+    <t>[Fysetc E4](https://www.fysetc.com/products/fysetc-e4-board-with-built-in-wi-fi-and-bluetooth-4-pcs-tmc2209-240mhz-16m-flash-3d-printer-control-board-based-for-3d-printer?variant=37558333341871)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=Fysetc%20E4%20v1.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Fysetc S6 V2](https://wiki.fysetc.com/FYSETC_S6/)</t>
+    <t>[Fysetc S6 V2](https://wiki.fysetc.com/FYSETC_S6/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Fysetc%20S6%20V2.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Mach 3 USB BOB - BSMCE04U-PP](https://embeddedtronicsblog.wordpress.com/2023/05/17/grbl-running-on-the-4-axis-bsmce04-pp/)&lt;sup&gt;1&lt;/sup&gt;</t>
+    <t>[Mach 3 USB BOB - BSMCE04U-PP](https://embeddedtronicsblog.wordpress.com/2023/05/17/grbl-running-on-the-4-axis-bsmce04-pp/)&lt;sup&gt;1&lt;/sup&gt;</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F1xx&amp;board=Mach3%20USB%20breakout%20%28BSMCE04U%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Makerbase MKS-DLC32 MAX](https://github.com/makerbase-mks/MKS-DLC32)</t>
+    <t>[Makerbase MKS-DLC32 MAX](https://github.com/makerbase-mks/MKS-DLC32)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=MKS%20DLC32%20MAX%20v1,%208MB+%20flash)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Makerbase MKS-DLC32](https://github.com/makerbase-mks/MKS-DLC32)</t>
+    <t>[Makerbase MKS-DLC32](https://github.com/makerbase-mks/MKS-DLC32)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=MKS%20DLC32%202.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Makerbase MKS-TinyBee](https://github.com/makerbase-mks/MKS-TinyBee)</t>
+    <t>[Makerbase MKS-TinyBee](https://github.com/makerbase-mks/MKS-TinyBee)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=MKS%20Tinybee%20V1.0)</t>
   </si>
   <si>
-    <t xml:space="preserve">[MKS SBASE v1.3](https://github.com/makerbase-mks/MKS-SBASE)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[MSP430F5529 LaunchPad](https://www.ti.com/tool/MSP-EXP430F5529LP) with [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
+    <t>[MKS SBASE v1.3](https://github.com/makerbase-mks/MKS-SBASE)</t>
+  </si>
+  <si>
+    <t>[MSP430F5529 LaunchPad](https://www.ti.com/tool/MSP-EXP430F5529LP) with [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
   </si>
   <si>
     <t>[MSP430F5529](https://github.com/grblHAL/MSP430F5529)</t>
   </si>
   <si>
-    <t xml:space="preserve">[MSP-EXP432E401Y LaunchPad](http://www.ti.com/tool/MSP-EXP432E401Y#) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
+    <t>[MSP-EXP432E401Y LaunchPad](http://www.ti.com/tool/MSP-EXP432E401Y#) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
   </si>
   <si>
     <t>[MSP432E401Y](https://github.com/grblHAL/MSP432E401Y)</t>
   </si>
   <si>
-    <t xml:space="preserve">[MSP-EXP432P401R LaunchPad](https://www.ti.com/tool/MSP-EXP432P401R) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
+    <t>[MSP-EXP432P401R LaunchPad](https://www.ti.com/tool/MSP-EXP432P401R) with  [CNC Boosterpack](https://github.com/terjeio/CNC_Boosterpack)</t>
   </si>
   <si>
     <t>[MSP432P401R](https://github.com/grblHAL/MSP432P401R)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [Arduino v3 shield](https://www.makerfabs.com/arduino-cnc-shield-v3.html)</t>
+    <t>[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [Arduino v3 shield](https://www.makerfabs.com/arduino-cnc-shield-v3.html)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Generic%20Uno/Nucleo-64%20%28STM32F411%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [CNC Breakout Nucleo64](https://github.com/terjeio/CNC_Breakout_Nucleo64)</t>
+    <t>[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [CNC Breakout Nucleo64](https://github.com/terjeio/CNC_Breakout_Nucleo64)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Nucleo-64%20CNC%20Breakout%20%28STM32F411%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [Protoneer v3 shield](https://blog.protoneer.co.nz/arduino-cnc-shield/)</t>
+    <t>[Nucleo F411RE](https://www.st.com/en/evaluation-tools/nucleo-f411re.html) with [Protoneer v3 shield](https://blog.protoneer.co.nz/arduino-cnc-shield/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Protoneer%20v3/Nucleo-64%20%28STM32F411%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [Arduino v3 shield](https://www.makerfabs.com/arduino-cnc-shield-v3.html)</t>
+    <t>[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [Arduino v3 shield](https://www.makerfabs.com/arduino-cnc-shield-v3.html)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Generic%20Uno/Nucleo-64%20%28STM32F446%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [CNC Breakout Nucleo64](https://github.com/terjeio/CNC_Breakout_Nucleo64)</t>
+    <t>[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [CNC Breakout Nucleo64](https://github.com/terjeio/CNC_Breakout_Nucleo64)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Nucleo-64%20CNC%20Breakout%20%28STM32F446%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [Protoneer v3 shield](https://blog.protoneer.co.nz/arduino-cnc-shield/)</t>
+    <t>[Nucleo F446RE](https://www.st.com/en/evaluation-tools/nucleo-f446re.html) with [Protoneer v3 shield](https://blog.protoneer.co.nz/arduino-cnc-shield/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=Protoneer%20v3/Nucleo-64%20%28STM32F446%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[OpenBuilds BlackBox X32](https://openbuildspartstore.com/BlackBox-Motion-Control-System-X32)</t>
+    <t>[OpenBuilds BlackBox X32](https://openbuildspartstore.com/BlackBox-Motion-Control-System-X32)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=BlackBox%20X32)</t>
@@ -259,7 +263,7 @@
   <si>
     <r>
       <rPr>
-        <u val="single"/>
+        <u/>
         <sz val="11"/>
         <color indexed="64"/>
         <rFont val="Calibri"/>
@@ -279,40 +283,37 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=PiBot%206-axis%20I2S)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Pi Pico](https://www.raspberrypi.org/products/raspberry-pi-pico/) on [PicoCNC](https://github.com/phil-barrett/PicoCNC)</t>
+    <t>[Pi Pico](https://www.raspberrypi.org/products/raspberry-pi-pico/) on [PicoCNC](https://github.com/phil-barrett/PicoCNC)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=RP2040&amp;board=PicoCNC)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Protoneer v3](https://blog.protoneer.co.nz/arduino-cnc-shield/) on ESPDuino</t>
+    <t>[Protoneer v3](https://blog.protoneer.co.nz/arduino-cnc-shield/) on ESPDuino</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=ESPDUINO-32%20Wemos%20D1%20R32)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Radds 1.6](https://reprap.world/electronics/development_boards/radds_v1_6_pre_assembled_3d_printer_board/)</t>
+    <t>[Radds 1.6](https://reprap.world/electronics/development_boards/radds_v1_6_pre_assembled_3d_printer_board/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=SAM3X8E&amp;board=Radds%201.6)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Re-ARM board](https://www.panucatt.com/Re_ARM_for_RAMPS_p/ra1768.htm) with [Ramps 1.6](https://reprap.org/wiki/RAMPS_1.6)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Sienci Labs SuperLongBoard Ext](https://sienci.com/product/slb/)</t>
+    <t>[Re-ARM board](https://www.panucatt.com/Re_ARM_for_RAMPS_p/ra1768.htm) with [Ramps 1.6](https://reprap.org/wiki/RAMPS_1.6)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=SuperLongBoard%20External%20%28SLB%20EXT%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Sienci Labs SuperLongBoard](https://sienci.com/product/slb/)</t>
+    <t>[Sienci Labs SuperLongBoard](https://sienci.com/product/slb/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32F4xx&amp;board=SuperLongBoard%20%28SLB%29)</t>
   </si>
   <si>
-    <t xml:space="preserve">[SMART Ramps](https://reprap.org/wiki/SMART_RAMPS)</t>
+    <t>[SMART Ramps](https://reprap.org/wiki/SMART_RAMPS)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=SAM3X8E&amp;board=Ramps%20SMART)</t>
@@ -327,16 +328,16 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=SourceRabbit%204-axis%20CNC)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Spark Concepts xPro v5](https://www.spark-concepts.com/cnc-xpro-v5/)</t>
+    <t>[Spark Concepts xPro v5](https://www.spark-concepts.com/cnc-xpro-v5/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=ESP32&amp;board=xPro%20v5)</t>
   </si>
   <si>
-    <t xml:space="preserve">[STM32F401CCU6 UNI](https://github.com/Am0k-GIT/STM32F401CCU6_UNI)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Teensy 4.0](https://www.pjrc.com/store/teensy40.html) on [T40X101](https://github.com/phil-barrett/grbl-teensy-4)</t>
+    <t>[STM32F401CCU6 UNI](https://github.com/Am0k-GIT/STM32F401CCU6_UNI)</t>
+  </si>
+  <si>
+    <t>[Teensy 4.0](https://www.pjrc.com/store/teensy40.html) on [T40X101](https://github.com/phil-barrett/grbl-teensy-4)</t>
   </si>
   <si>
     <t>[iMXRT1062](https://github.com/grblHAL/iMXRT1062)</t>
@@ -345,52 +346,61 @@
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=iMXRT1062&amp;board=T40X101)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [E5XMCS_T41](https://www.makerstore.com.au/product/elec-e5xmcst41/)</t>
+    <t>[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [E5XMCS_T41](https://www.makerstore.com.au/product/elec-e5xmcst41/)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=iMXRT1062&amp;board=E5XMCS_T41)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [GRBLHAL2000](https://github.com/Expatria-Technologies/grblhal_2000_PrintNC)</t>
+    <t>[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [GRBLHAL2000](https://github.com/Expatria-Technologies/grblhal_2000_PrintNC)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=iMXRT1062&amp;board=GRBLHAL2000%20-%20PRINTNC)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [T41BB5X_PRO](https://github.com/phil-barrett/grbl-teensy-4)</t>
+    <t>[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [T41BB5X_PRO](https://github.com/phil-barrett/grbl-teensy-4)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=iMXRT1062&amp;board=T41BB5X%20Pro)</t>
   </si>
   <si>
-    <t xml:space="preserve">[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [T41U5XBB](https://github.com/phil-barrett/grbl-teensy-4)</t>
+    <t>[Teensy 4.1](https://www.pjrc.com/store/teensy41.html) on [T41U5XBB](https://github.com/phil-barrett/grbl-teensy-4)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=iMXRT1062&amp;board=T41U5XBB)</t>
   </si>
   <si>
-    <t xml:space="preserve">[WeAct Blackpill](https://github.com/WeActTC/MiniF4-STM32F4x1) on a [Minimal breakout](https://github.com/avizienis/Minimal-Black-Pill--STM32F4xx-BOB-for-grblHAL)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[WeAct MiniSTM32H7xx](https://github.com/WeActTC/MiniSTM32H7xx)</t>
+    <t>[WeAct Blackpill](https://github.com/WeActTC/MiniF4-STM32F4x1) on a [Minimal breakout](https://github.com/avizienis/Minimal-Black-Pill--STM32F4xx-BOB-for-grblHAL)</t>
+  </si>
+  <si>
+    <t>[WeAct MiniSTM32H7xx](https://github.com/WeActTC/MiniSTM32H7xx)</t>
   </si>
   <si>
     <t>[WebBuilder](https://svn.io-engineering.com:8443/?driver=STM32H7xx&amp;board=WeAct%20Mini%20H743)</t>
+  </si>
+  <si>
+    <t>[Sienci Labs SuperLongBoard Ext](https://sienci.com/product/slb-ext-closed-loop-controller/)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.000000"/>
+      <sz val="11"/>
+      <color indexed="64"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color indexed="64"/>
       <name val="Calibri"/>
     </font>
@@ -405,20 +415,20 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -431,295 +441,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -924,23 +654,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C57"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="100" workbookViewId="0">
-      <selection activeCell="C9" activeCellId="0" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="128.28515625"/>
-    <col customWidth="1" min="2" max="2" width="49.42578125"/>
+    <col min="1" max="1" width="128.28515625" customWidth="1"/>
+    <col min="2" max="2" width="49.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -948,7 +680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -959,7 +691,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -967,7 +699,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -978,7 +710,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -989,7 +721,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -1000,7 +732,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -1011,7 +743,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +754,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1033,7 +765,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -1044,7 +776,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -1055,7 +787,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" s="1" customFormat="1">
+    <row r="12" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
@@ -1066,7 +798,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1077,7 +809,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>31</v>
       </c>
@@ -1085,7 +817,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="15" s="1" customFormat="1">
+    <row r="15" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>33</v>
       </c>
@@ -1093,7 +825,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>34</v>
       </c>
@@ -1104,7 +836,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -1112,7 +844,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>38</v>
       </c>
@@ -1120,7 +852,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>40</v>
       </c>
@@ -1131,7 +863,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>42</v>
       </c>
@@ -1142,7 +874,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>44</v>
       </c>
@@ -1153,7 +885,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>46</v>
       </c>
@@ -1164,7 +896,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
@@ -1175,7 +907,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>50</v>
       </c>
@@ -1186,7 +918,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="25" s="1" customFormat="1">
+    <row r="25" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>52</v>
       </c>
@@ -1197,7 +929,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>54</v>
       </c>
@@ -1208,7 +940,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="27">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>56</v>
       </c>
@@ -1219,7 +951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>58</v>
       </c>
@@ -1227,7 +959,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>59</v>
       </c>
@@ -1235,7 +967,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>61</v>
       </c>
@@ -1243,7 +975,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -1251,7 +983,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>65</v>
       </c>
@@ -1262,7 +994,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>67</v>
       </c>
@@ -1273,7 +1005,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -1284,7 +1016,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>71</v>
       </c>
@@ -1295,7 +1027,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>73</v>
       </c>
@@ -1306,7 +1038,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -1317,7 +1049,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>77</v>
       </c>
@@ -1328,7 +1060,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>79</v>
       </c>
@@ -1339,7 +1071,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>81</v>
       </c>
@@ -1350,7 +1082,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>83</v>
       </c>
@@ -1361,7 +1093,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="42">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>85</v>
       </c>
@@ -1372,7 +1104,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="43">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>87</v>
       </c>
@@ -1380,190 +1112,182 @@
         <v>32</v>
       </c>
     </row>
-    <row r="44" s="1" customFormat="1">
+    <row r="44" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C44" s="1" t="s">
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="1" t="s">
+      <c r="B45" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" t="s">
         <v>90</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C45" t="s">
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>91</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="s">
-        <v>92</v>
       </c>
       <c r="B46" t="s">
         <v>6</v>
       </c>
       <c r="C46" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
-        <v>94</v>
       </c>
       <c r="B47" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="48">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B48" t="s">
         <v>3</v>
       </c>
       <c r="C48" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>96</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="s">
-        <v>97</v>
       </c>
       <c r="B49" t="s">
         <v>3</v>
       </c>
       <c r="C49" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="s">
+      <c r="B50" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>99</v>
       </c>
-      <c r="B50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="s">
+      <c r="B51" t="s">
         <v>100</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>101</v>
       </c>
-      <c r="C51" t="s">
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="s">
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" t="s">
         <v>103</v>
       </c>
-      <c r="B52" t="s">
-        <v>101</v>
-      </c>
-      <c r="C52" t="s">
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="s">
+      <c r="B53" t="s">
+        <v>100</v>
+      </c>
+      <c r="C53" t="s">
         <v>105</v>
       </c>
-      <c r="B53" t="s">
-        <v>101</v>
-      </c>
-      <c r="C53" t="s">
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="s">
+      <c r="B54" t="s">
+        <v>100</v>
+      </c>
+      <c r="C54" t="s">
         <v>107</v>
       </c>
-      <c r="B54" t="s">
-        <v>101</v>
-      </c>
-      <c r="C54" t="s">
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="s">
+      <c r="B55" t="s">
+        <v>100</v>
+      </c>
+      <c r="C55" t="s">
         <v>109</v>
       </c>
-      <c r="B55" t="s">
-        <v>101</v>
-      </c>
-      <c r="C55" t="s">
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="s">
+      <c r="B56" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
         <v>111</v>
-      </c>
-      <c r="B56" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="s">
-        <v>112</v>
       </c>
       <c r="B57" t="s">
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:C57">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C57">
     <sortCondition ref="A2:A57"/>
   </sortState>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView zoomScale="100" workbookViewId="0">
-      <selection activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
-  <printOptions headings="0" gridLines="0"/>
-  <pageMargins left="0.69999999999999996" right="0.69999999999999996" top="0.75" bottom="0.75" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
-  <headerFooter/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>